<commit_message>
Get daily reddit data: Tue Nov 28 08:08:34 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_03.xlsx
+++ b/data/2023_12_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C443"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2420 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>185qx8w</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Love my nails!!!!</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4uz40xjvp13c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>185qv2k</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>My long black nails</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sxhkehx8p13c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>185qmg1</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/185qmg1/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>185q3xc</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Red with glitter, in real life looks more dark</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kntgzohuf13c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>185ppjo</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Best nails to use?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/185ppjo/best_nails_to_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>185pgar</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>I am yet to finish nail school. How did I do?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngkuyp17813c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>185npbj</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Girlfriend made this</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/re181kh4p03c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>185mvk9</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aega56v2h03c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>185mqsa</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>i love a nice nude nail color 💕</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0mbzlfsf03c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>185mglt</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>my favorite red🍷</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185mglt</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>185mbj7</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Recommendations for e-file</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/185mbj7/recommendations_for_efile/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>185m7ds</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye Christmas nails! </t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/19kzf38wa03c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>185m4o5</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>🌞 ILNP Quicksand ✨ I needed a neutral palette cleanser before the holidays 🤎</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185m4o5</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>185lxc8</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>What's your pedicure/foot care routine?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1bw197ve803c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>185lt4m</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Would these look good with pink glitter instead of gold?</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twq8yehj703c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>185l9zs</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Festive nails!</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdyl0odv203c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>185l0q3</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Help with my nail shape !!!!</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185l0q3</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>185ktgn</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>help! what red nails do i get for december?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6u483vyyz2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>185kb84</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>which ones do you like more?</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185kb84</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>185k7jq</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Mood changing gel polish</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185k7jq</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>185jx1n</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Need nail salon recommendations</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/185jx1n/need_nail_salon_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>185jt23</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>How can I improve?</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fa88y5reqz2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>185jiy3</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>My first full set of diy acrylics</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dy9nm4b3oz2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>185j7ei</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>My new nails I love them</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ob846qbclz2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>185irzx</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Are my nail beds long?</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxzp9zruhz2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>185iqp7</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Is it obvious they’re press ons?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/11pnce8lhz2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>185ih1z</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Holiday Nails 💚</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185ih1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>185idbo</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>A little something for December</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rua8z72oez2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>185es3c</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Need birthday inspo!!</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/185es3c/need_birthday_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>185hmgv</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Swatches of my Zoya haul 🩷</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8y48u2lx8z2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>185gh1y</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>27/11/2023: Apologies for the bad drawing, but why do nail techs do this/why does this happen? I’ve seen it many times before on acrylics and even press-ons, is it done on purpose? I know nothing of acrylics, so maybe I’m misunderstanding something here. Thanks in advance.</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9d5ophsc0z2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>185ftkt</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>gel nails never last</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/185ftkt/gel_nails_never_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>185ff9x</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>My nail lifted and came clean off after 1 week. Bummed.</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185ff9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>185e2k4</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>What causes this?</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xsnwuheajy2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>185e80p</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Biab nails???</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/185e80p/biab_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>185e44o</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>2 months of growth. Cold turkey stopped biting and my nail beds are healing ❤</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185e44o</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>185dd0n</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>What do we think of this set y’all?</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185dd0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>185dad1</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Super beautiful💕</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8i9wpkrdy2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>185bcsf</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>How to repair a cracked nail?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185bcsf</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>185cpg2</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>It’s my birthday! I don’t usually get nail art done, but I think these are cute</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjz45msk9y2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>185cfs3</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Tips for extending nail wraps?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwpmqi5l7y2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>185c88z</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Christmas Nails! 🎄⛄️🎅❄️</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185c88z</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>185bvvn</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>A moment of silence</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185bvvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>185btxg</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>My nails have never been harder to bite off after taking collagen for 2 months</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/185btxg/my_nails_have_never_been_harder_to_bite_off_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>185bssw</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>First Christmas nails of the season!</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/95x206ft2y2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>185b7ft</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>How to fix too much chrome?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwy0odleyx2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>185a0zx</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>CND vs OPI for wear time</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/185a0zx/cnd_vs_opi_for_wear_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1859ynu</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Simple but cute</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ajybgaoapx2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1858wkw</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Tried the holo powder on my poor nails</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jinjdicqhx2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1858gb3</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>its timeeeeeeeee</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bnfgaaudex2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>185821v</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Hand painted oddities nails</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185821v</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1857iyg</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Iridescent joy!</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1857iyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>18576en</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Red ♥️</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ttv8mi35x2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>18569lo</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Started doing builder gel + extensions a few months ago; just some stuff I’ve done!🥰(newest to oldest)</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18569lo</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1855zbj</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>I love these!</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jfuxwzjyvw2c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>184zzej</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>What kind of manicure should you get for a one-off?</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/184zzej/what_kind_of_manicure_should_you_get_for_a_oneoff/</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>184xrdu</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Help! Whenever I do top coat the sides are always sticky</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4i3wmv6iju2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>184xake</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Need help finding a nail polish color</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d9k8z9hkdu2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1855bky</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>My bio gel is lifting after a week??</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1855bky</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1854oe4</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Having issues with madam glam</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1854oe4/having_issues_with_madam_glam/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1853z1i</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Got my nails done recently by @piopionails on ig~💅🏻</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1853z1i</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1853j2c</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Pre-holiday nails ❄️</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygsq0a45cw2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1852zns</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>most elaborate set I've ever had 💙</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0f47dv07w2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1852nta</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Super beautiful😍</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1852nta</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1852asx</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>As Christmassy as it’s going to get</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1fpxaebs0w2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1850trs</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>How to stop picking dead skin around my nails</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1850trs</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1850awd</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Nail foils and Holo powder</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/scx11h4efv2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>184yvj4</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/184yvj4</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>184yrn1</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Press-Ons I made for my sister</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0i4x1zbawu2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>184v7zb</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Super Late Halloween Nails</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upwxoxl8qt2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>185q6of</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>I love fancy neutrals ✨</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1k95dy9rg13c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>185psvc</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Zoya Patrice</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/790thcx5c13c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>185oy0h</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Nail polish named "Esther" or "Joe"??</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/185oy0h/nail_polish_named_esther_or_joe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>185nmsn</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>The search for a red I like is over! I created it with Orly Color Labs</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nl4cbheeo03c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>185nh8c</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>A little autumn shiftiness!</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185nh8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>185ml8i</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Eyelid Irritation from Nail Polish</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/185ml8i/eyelid_irritation_from_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>185m38z</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>🌞 ILNP Quicksand ✨ I needed a neutral palette cleanser before the holidays 🤎</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185m38z</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>185lwkr</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>1st day at new job tomorrow mani.</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9p7jxoeb803c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>185lbbh</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>When you all refer to “indy polishes” what brands are you referring to?</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/185lbbh/when_you_all_refer_to_indy_polishes_what_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>185l3sm</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>What to do with duplicate shades?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185l3sm</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>185kty4</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>this polish is too pretty🤩</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185kty4</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>185kqdv</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Golden hour holo 😍</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185kqdv</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>185kfwa</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>In love with first thermal</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yclb8xdnvz2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>185k1p6</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Ethereal Crescent City: Ruhndanaan and Hunt, corresponding mysteries, + GWP.</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185k1p6</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>185k1hc</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Perfect fall to winter transition polish</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lubx6l7dsz2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>185j36s</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>🍁🍂 Last Fall Manicure of the season 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185j36s</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>185irgj</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>First set I did on myself</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185irgj</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>185ikpg</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Opinions? First time trying to give myself a pedi all alone. Be honest it won’t hurt my feelings :)</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1trmxc2agz2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>185ijgr</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Neutral-ish skittle</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185ijgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>185iiu8</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Destashed on Buy Nothing Group!</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/185iiu8/destashed_on_buy_nothing_group/</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>185id32</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Thoughts on Builder Gel?</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6u4377xlez2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>185i8ji</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>mermaid bait to combat the cold✨</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185i8ji</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>185hz1x</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Can you cure a gel top coat on regular nail polish?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/185hz1x/can_you_cure_a_gel_top_coat_on_regular_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>185hvtg</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Brightening up my fall :)</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185hvtg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>185hu8n</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Like literal pearls on my nails ⚪</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pg9pntmlaz2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>185h4p3</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>DIY Cuticle Oil</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/185h4p3/diy_cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>185grko</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Similar formulas to KBShimmer's Come As You Are ?</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehi5gf3h2z2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>185fh58</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>New to painting my nails</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185fh58</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>185fat7</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Nail biter going nail painter. Started with red and everytime one chips I'm adding to my chaotic Christmas manicure instead of biting. Hope they grow long.</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oluflzptry2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>185f20k</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>I can’t stop staring at this one 😍</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lu90gch5qy2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>185dj22</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Le Mini Macaron - Smoky Matcha</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xc29xuukfy2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>185dgml</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>A rant about Cirque brushes</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omonyim2fy2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>185d5bn</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Cool Cat Mom is unexpectedly gorgeous!!!</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wxl6cfzncy2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1858zzc</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>A gorgeous deep green</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i51p9aveix2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>185d0l3</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Squeezing in the last few days of fall manis</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185d0l3</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>185cn10</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>cock_a_doodle_doom</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185cn10</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>185bhqv</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Zoya Mae</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185bhqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>185a63c</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>I was journaling and caught Flight of the Monarchs doing its thing 🥹</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o651dg6tqx2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>185a598</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Velvet hack q - why did my topcoat ruin it?</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hr8wz3wmqx2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1859sln</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>When the warehouse lighting hits 💅</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1l1rv83ox2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>18597ph</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Mooncat Access Denied! Finally stopped biting my nails but now I need to stop picking off polish 😭</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18597ph</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>18585d2</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Swatch Question</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18585d2/swatch_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>18583o9</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>ILNP Rosewater</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqv8h10ybx2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1857u58</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>How to prep nails for painting over existing lacquer?</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1857u58/how_to_prep_nails_for_painting_over_existing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1856w6c</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>RIP to my long nails, hello short squares 🔳</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/he0r23et2x2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1856se9</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>your favorite "no-polish" polish?</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1856se9/your_favorite_nopolish_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1856ktv</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Jojoba oil</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1856ktv/jojoba_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1856ebf</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Nude snake skin</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0b9z12u7zw2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1856d3e</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Holly Jolly</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ryrhuwyyw2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>18569e8</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Sparkly neutral winter manicure</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9vx1bx6yw2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>18564sf</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>My MIL complimented my nails on Thanksgiving, officially buying Mooncat forever 😂</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18564sf</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1855ezb</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>I coincidentally bought a polish that matches my coat</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1855ezb</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1855brz</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>First time trying a cat eye</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/inwvc3irqw2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1855404</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Question about press ons</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1855404/question_about_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>18551bd</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Weekly check-in for those on a low buy, no buy, etc. [POST-BLACK FRIDAY EDITION]</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18551bd/weekly_checkin_for_those_on_a_low_buy_no_buy_etc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1854wpd</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Can you find magnetic nail polish in stores?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1854wpd/can_you_find_magnetic_nail_polish_in_stores/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1854lrx</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>I have defeated many indie temptations with this drugstore polish</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lb2tp6xykw2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>18547i9</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Covid got me, but at least I have this polish</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18547i9</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1853ukz</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Pink</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ete3xkbsew2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>18534dj</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Nail varnish that doesn't match the Swatch/description</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hna120te8w2c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1853273</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Quick video of cat eye with Clionadh Psilocybin</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/abz93hhu7w2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1850fhk</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1850fhk/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>184ytw6</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>I’m legit gonna cry 🥲</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/184ytw6</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>184yrwd</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Confirming that Cirque Blue Velvet is super pretty velvetized💙</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6jihdrqcwu2c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>185q4yk</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>My new red nails with glitter</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185q4yk</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>185puu8</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Working on my holiday nails!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5b4oq6vc13c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>185m5zj</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Cat eye Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qvqtcm4ka03c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>185l6qx</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Anyone have an idea what polish was used here or which foil?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/185l6qx/anyone_have_an_idea_what_polish_was_used_here_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>185jon4</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Design according to the client's opinion</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jwahp2fpz2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>185imcq</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>halloween design made by me</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6w8zfomgz2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>185fncc</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>🤎</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185fncc</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>185aikr</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Fruity</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trq3lractx2c1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Nov 29 08:08:42 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_03.xlsx
+++ b/data/2023_12_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C443"/>
+  <dimension ref="A1:C596"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7964,6 +7964,2607 @@
         </is>
       </c>
     </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>186jhvc</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Christmas claws</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1aab0j1k83c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>186jdnz</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>😩</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7zz697mi83c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>186iql4</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Digging this purple</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ey9gc24jb83c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>186indz</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Does this color fit me?</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186indz</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>186hnib</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>latest custom press on</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aarx0ehe083c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>186h981</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>What is a good Christmas gift idea for my nail tech(s)?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/186h981/what_is_a_good_christmas_gift_idea_for_my_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>186fibq</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Jello Jello Peel off base?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/186fibq/jello_jello_peel_off_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>186h4ng</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>First time posting 💅🏻</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186h4ng</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1868eu1</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>It’s me again! Hi! 🙈 😂 💅</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1868eu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>186h2d6</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Crying Lightning</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgcajaoku73c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>186h1t8</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Best nail shape/type if you work using your hands all day? (I’m a florist)</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/186h1t8/best_nail_shapetype_if_you_work_using_your_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>186gwjz</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>natural nails with dip</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186gwjz</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>186gsm9</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>My insanely long natural nails !</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tes66i6zr73c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>186g2zr</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>My beautiful nails as a graduation present</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186g2zr</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>186g0o3</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>I don't get my nails done often because I don't want them to prevent me from gaming, but I could not help myself. They were too cute &lt;3</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x01t7e5mk73c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>186fupq</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>New to Nail Art!</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186fupq</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>186eqt5</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>new set !</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9r3rxp1ea73c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>186ehxv</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Simple nails are my fave</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bo9325ec873c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>186ecnd</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Fresh Mani</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186ecnd</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>186e6tz</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Got a job interview tomorrow and went with these</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6gxw60t573c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>186c1s0</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Hybrid gel?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/186c1s0/hybrid_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>186d4ol</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Matchy matchy</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bimks854x63c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>186d2mw</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Going to the Renaissance movie Thursday and had to get festive lol 🪩</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13j0dhqow63c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>186ctp0</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Look at that shine!</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186ctp0</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>186cd9r</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Chronic nail picker here 👋🏼 Wanted to share my first manicure in years. So happy with it!</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ap5cb39tq63c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>186ca6g</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Did the nail place screw me over?</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186ca6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>186c8gy</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>dnd gel question</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/186c8gy/dnd_gel_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>186c0bt</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Saw Nails that I did months ago 💅🏻😍</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dq9f5rhzn63c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>186bocm</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>i saw someone else post their natural nails. here’s mine✨</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186bocm</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>186bakz</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Solid Sterling Silver Press on Nails</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186bakz</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>186b3qr</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>nail polish keeps chipping, help!</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/186b3qr/nail_polish_keeps_chipping_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>186atxk</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>im all wrapped up! 🎄🎁🫶🏽✨</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186atxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1868t48</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Holiday light nails</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbgp1qb1063c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1868kj0</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Married, separated 😂</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1868kj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1868733</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>First time with nail art</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8rjim5nvv53c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>186807h</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Special “add on” for holidays</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/186807h/special_add_on_for_holidays/</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1864dzj</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Inspired by some polishes I saw recently so decided to try and dupe.</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udj68t15453c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1860wqy</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>My first holiday set</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1860wqy</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1867k8x</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Gel X method &amp; transfer foils</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1867k8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>185mojs</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Why do my nude manicures become darker over time?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12nj5826f03c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>18678iz</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>DIY Manicure</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnp5wb70p53c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1866uqx</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Do we accept natural nails? 🫣</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7388qcllm53c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1866sd8</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Are Gel X type extensions very good for wavy/mishapen nails?</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2uglgz4m53c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>18662dy</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>New set by me</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18662dy</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1865zuc</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Sugar nail design help</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1865zuc/sugar_nail_design_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1865dr7</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>First set of Christmas nails</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1865dr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1865776</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>I’ve been growing my nails for 6 months now</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1865776</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>18654b8</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oz283olk953c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>186544f</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Summertime!</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ri54n52j953c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>18647xm</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Showing some natural nails here!</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzqmwg8w253c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>18641w6</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>I did some wintery themed nails (air dry)</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18641w6</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1863nmz</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>proud of myself</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1863nmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>18639g8</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Gel x and cleaning products</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18639g8/gel_x_and_cleaning_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1862u07</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Going to Disney in 2 days. Obviously had to get the minimalistic Mickey ❤️</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/59t99umps43c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>18628u9</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Barbie Pink Christmas Fantasy🥹🩷 my nail tech is the best!!</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18628u9</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>186282r</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Christmas Lights ✨️</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186282r</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>18624x2</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Good UV Gel polish brand recommendations</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18624x2/good_uv_gel_polish_brand_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1861dv5</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>nondominant hand</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1861dv5/nondominant_hand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>18612sn</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Builder gel and product compatibility</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18612sn/builder_gel_and_product_compatibility/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1860z2q</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>good thing my next appointment is in a week :’)</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1eyo5tsse43c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1860qsl</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Chrome powder on my natural nails</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0y2dmyr3d43c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1860hld</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>RED Christmas nails🎄</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1860hld</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>185zm6k</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185zm6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>185zj7h</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Nail adhesive suggestions for full-cover soft gel tips?</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/185zj7h/nail_adhesive_suggestions_for_fullcover_soft_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>185yzm2</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>I love these nails 💅🏼😍</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjdvbaoyz33c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>185yvc9</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>New claws 🌸🌸🌸</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ynpf6kjzy33c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>185ys62</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Nailtastic</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0jbw5qcy33c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>185ylk2</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>christmas time equals sparkle</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myl2qutyw33c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>185yjl7</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Green for Christmas 🤔</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fn6cb93kw33c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>185ya09</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>This is my first time getting my Nails painted. I want my feet to look more feminine but i am getting anxious because i don’t think they do .. does the color go well with my skin ?</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fu0zp0zdu33c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>185y3fe</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Sailor Moon Nails 🌙</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvxvqtlvs33c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>185xlgt</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Absolutely in love with these😍</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hgtkk6wuo33c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>185xe7m</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Sweater Nails🩶🩷🤍</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yq6sagr6n33c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>185x59r</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>all of the nail salons around me charge so much for fills, I don’t even know where to go lol.</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/185x59r/all_of_the_nail_salons_around_me_charge_so_much/</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>185vy3g</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>DIY gel with stamping</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0yrzix15b33c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>185vgq7</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Christmas nails and gel</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psl9idgq633c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>185v1bl</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Finding good salons can be hard when traveling!</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185v1bl</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>185thoy</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Went to the nail salon for the first time and I love love love how these turned out &lt;3</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wl1tf97ql23c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>185syat</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Oval (almond? Which is the red?) or coffin shape…which is more flattering? I used to love the first, that red with that shape every fill. Started up with coffin shape and stayed with it til they came off over a year ago. Seems like growing them healthy is sorta hard.😅 product question too👇🏼👇🏼👇🏼</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185syat</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>185sj41</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>paid £25 for this set… not sure if i should ask for a refund. did i get what i paid for?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgg5z698a23c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>185rmbq</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Presson</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185rmbq</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>185riiw</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>My nails I got recently. Chrome tips on a pink base.</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185riiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>185r64v</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>No lift - I just love IT</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185r64v</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>186keak</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>PROs and CONs about Paddie’s starter kit</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/186keak/pros_and_cons_about_paddies_starter_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>186k72z</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>On a topper kick ✨</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186k72z</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>186j3y5</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Shouldn’t have slept on “not today satan” she’s a stunner!!!</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3fnek16hf83c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>186i6ar</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Palette cleanser color</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pa7smxpm583c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>186hsdu</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>What is the hottest pink polish out there?</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/186hsdu/what_is_the_hottest_pink_polish_out_there/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>186g6zs</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Skittle mani feat. Lacquer22 BF haul</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzh2p5ccm73c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>186gt0d</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Finally can do a decent checkers after a ton of practice!</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yaedflnr73c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>186gg54</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Just the most fun I’ve ever had sponging something onto something else</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186gg54</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>186g8w2</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>First time ombre nails 🦋🦄✨</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ynzg1mptm73c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>186fjk2</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Going to Vegas and getting my nails done for the first time, could use some recs!</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/186fjk2/going_to_vegas_and_getting_my_nails_done_for_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>186ejbg</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Quick Dry Top Coat Refill recommendation without harmful ingredients</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/186ejbg/quick_dry_top_coat_refill_recommendation_without/</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>186db6o</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>What do i need to build a good structure on a real nail + materials</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/186db6o/what_do_i_need_to_build_a_good_structure_on_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>186d64r</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Dark Galaxy Lava Vibes</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186d64r</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>186b08n</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Did ILNP take off thepolishedyogi off their list? And creator suggestions</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/186b08n/did_ilnp_take_off_thepolishedyogi_off_their_list/</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>186avx4</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>im all wrapped up! 🎄🎁🫶🏽✨</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186avx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>186a9jf</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Hopping on the velvet magnet hack 🧲</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lzize4zia63c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1868rcb</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>My Melody! 🩷</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rx8g779pz53c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1868nk5</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Finding old friends after a swatch project.</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1868nk5</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1868lro</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>How many, he asks? None of my business tbh.</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fpvve6ffy53c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1868kia</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>H&amp;M - Beyond Midnight + Poparazzi - Star Shine</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1868kia</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1867sk7</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Jelly mishmash turned out to be my perfect blue</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnxao6s3t53c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1867sge</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>What fun and surprising things destroy your mani?</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1867sge/what_fun_and_surprising_things_destroy_your_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1867owx</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Finally tried Lincoln Park After Dark</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8itkm00es53c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>185vaz3</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Self-manicures for mental health.</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185vaz3</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1867imr</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>OPI Sunrise...Bedtime! Dupe please?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1867imr</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>185njnw</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Newbie laquerista</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fkk0dp0kn03c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1867fco</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>🌵🍐</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1867fco</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1866waz</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Mooncat: Access Denied</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1866waz</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1866d4r</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Night Owl Flesh Of A Zombie</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1866d4r</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1866018</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Nail polish storage- IKEA and Container Store</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1866018</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1865qbh</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>How do you organize your swatches? I made a book.</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1865qbh</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1865ke2</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Fountain pen fans: inks like ILNP’s Eclipse?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1865ke2/fountain_pen_fans_inks_like_ilnps_eclipse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1864qr3</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>(Ethereal) Rhun Mystery Bag</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/z4SmRSU</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1863wnl</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Vanessa Molina Fishnet Stockings x KB shimmer No Illusions</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4wem6swk053c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1863mkh</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Holo Taco?</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1863mkh/holo_taco/</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1863dnb</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Update: polish on less than 2 days. Burnt my nail and it split and snagged on my pants :&lt;</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1863dnb</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1862yv0</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>yet another cock a doodle doom post</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bo0z62hpt43c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1862tm6</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Peas and Carrots!!</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3fm7x2wms43c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1862rcd</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>{PR} Roulette by ILNP 😍</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2qlnosi6s43c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1862i3b</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Just then...tragedy struck...</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sptkgof9q43c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>18625eu</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Ogres are like Onions 🧅</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/30s9thmon43c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1861zgk</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Purple Magenta shimmer polish from Dollar Tree!</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1861zgk</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1861uqv</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>I love these glowy shimmer sheers - Nov PPU Pahlish Mad Woman</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1861uqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1861bs6</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Got my Starrily order, immediately wanted to try velvet w/ "Hera"</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/usu6f88bh43c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>18610vn</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Hunt! 🩶💜🌙</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18610vn</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>186024t</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Shout out to Daveen Lacquer's customer service!</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dm82umlw743c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>185zt80</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>First Christmas mani of the season 🍬</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185zt80</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>185zkvd</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Mouthwash for nails</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185zkvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>185yiw2</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Cirque Colors - Velvet Rope ❤️</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oezdg4new33c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>185y15a</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>My Kind of Neutral</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185y15a</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>185xvaa</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Actual Nubby Nails</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xm3n6rr3r33c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>185xg6o</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>First time all different colors (with and without flash)</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185xg6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>185x1fx</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Last fall set 🍁</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9uif1xbk33c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>185tn0i</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Essie spaghetti strap</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g6l6h2den23c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>185tjs0</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Shimmer Accents on Navy</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/185tjs0</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>186ka7z</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>First Christmas set🎄</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186ka7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>186jndd</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Christmas design</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmlepn7yl83c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>186iukx</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>What is your favorite for this Christmas? 1,2,3? Let me know in the comments and support with an upvote (my favorite is number 2)</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186iukx</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>186i2k5</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>❄️ Gingerbread/Snowflake Nail Art ❄️</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jeonucek483c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>186gpve</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Star Wars Christmas Nails 💫💅🏼</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186gpve</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>186d322</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>My first attempt at a nail artpiece so it's quite rough (be gentle). I went for the web series ENA</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186d322</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>186al01</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Rainbow zebra stripes!</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n02ymggwc63c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1867ww2</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>How to not have gel top coat flake off full nail water slide decals?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1867ww2/how_to_not_have_gel_top_coat_flake_off_full_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1866vmw</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Practice Day 40, gel polish in resin molds</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sr29qvigm53c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1866mip</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>I feel like I will never get over these nails 🤡</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1866mip</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1864x24</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>First attempt ever at nail art after years of biting my nails.</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1864x24</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1864swn</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>My first time doing nails for my Girlfriend</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jstsiw03653c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1864hqn</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>🤎Gingerbread House🤎</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s6q5b35w453c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>185yaei</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Pollock Nails</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kc4ys2ihu33c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>185sol0</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>inspired by those cute viral cherry nails - some christmasish nailart 🎄</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/em5masc1c23c1.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Nov 30 08:08:31 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_03.xlsx
+++ b/data/2023_12_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C596"/>
+  <dimension ref="A1:C732"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10565,6 +10565,2318 @@
         </is>
       </c>
     </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>187d7ep</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>are nail charms mri safe? i have the ”vivienne westwood” charm and star charm with diamonds!! plzz helpp</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/187d7ep/are_nail_charms_mri_safe_i_have_the_vivienne/</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>187cxgz</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>I got her to add the red stripes today! Looks so much better</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oewqa2tbuf3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>187cpm5</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>What do you think of the color?.</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bty1lpkqrf3c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>187cl0y</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>When the nailpolish feeling kicks in...</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2a1i2v6qf3c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>187bwzp</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Pink French tips :)</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7762psvmif3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>187auy9</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Cow girl</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187auy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>187afdb</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Just had my first acrylic fill done yesterday and my pinky nail just snapped right off. Should the repair be free?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187afdb</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>187a80f</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Snowflakes one year apart</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187a80f</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>187a3n7</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Metallic Lavender Almond Frenchies 🥰</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6pop7ium0f3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1879ujo</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>My natural nails! (and I always do them myself, it’s one of my favorite hobbies)</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pfmm2gq9ye3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1879t1x</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Just a lil color pop 🪄</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2d657l7wxe3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1879guj</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Name of color</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l45hmmanue3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1878y9m</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Nails art</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzje2fhtpe3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1878v50</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Late fall | Nails matte vs shiney (excuse the non-oil-cuticles)</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1878v50</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1878o2b</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>It’s Christmas nail season</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9xjcfiy8ne3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1878hcu</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Got my nails done!</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdwfmx8mle3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1878dv3</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1878dv3</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1877t2i</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Tip adhesive instead of builder gel?</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1877t2i/tip_adhesive_instead_of_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1877imn</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>New witchy set</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1877imn</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1876uaf</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>ice princess nails ❄️</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1876uaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1876mpa</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Does square suit my hands?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6a9wdpk76e3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1876j5b</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Jelly Nails…?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1876j5b/jelly_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>18763y1</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Nails</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pn0ioc2x1e3c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>18760ur</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>cool glaze nail wraps 🧊</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18760ur</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1875kaw</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Do you agree that this nail color washes me out or am I wrong?</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1875kaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1875hfh</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Holiday Nails!!</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c12u5k5lwd3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1875fmp</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Silver Chrome Tips 🪙</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpfhtdm7wd3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1874xfz</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Practice hand for press ons</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1874xfz/practice_hand_for_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1874o5z</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Besties nail day</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i42tx37xpd3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1874aqn</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Mario &amp; Mario &amp; Sonic</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1874aqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>18745ip</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>I had a bad day, and asked for something happy and a little crazy. She delivered.</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blhjgaasld3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1872ovk</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ar22dnofad3c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1872bm3</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Taking breaks?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u6bl534l7d3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1871wtw</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Perfectly simple, love my new nails 🌻</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/99yql16h4d3c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1871q8v</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>The cutest baby nail oil!</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/savv2rm13d3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1871kye</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Do press-ons stay on better if your natural nails underneath are the same length?</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1871kye/do_pressons_stay_on_better_if_your_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1871kjg</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Artistic kitties</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m6dm6hdu1d3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1871577</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Black it is</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o3vu8p2nyc3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>18713ne</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>what design should i go for?</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18713ne/what_design_should_i_go_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1870yxj</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Hello! Why did my fake nail turned matte when I applied shiny top coat?</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1870yxj</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>187054t</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>ILNP Black Friday - delayed shipping???</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/187054t/ilnp_black_friday_delayed_shipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>186zuki</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186zuki</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>186zto5</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Girlfriend told me to get pretty for our date</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186zto5</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>186zf6y</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Seche Vive- apply on wet nails or dry?</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/186zf6y/seche_vive_apply_on_wet_nails_or_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>186yvwf</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Olive green under red pink chrome. Isn’t it interesting?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s67o0swdhc3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>186xqjx</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Nail shape?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186xqjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>186xnfi</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>2 years ago i grew out my nails for my wedding. Loved them but were so hard to maintain</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186xnfi</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>186x173</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Does it really matter??</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/186x173/does_it_really_matter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>186wwfg</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>time to get a new gel lamp &amp; need suggestions</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/186wwfg/time_to_get_a_new_gel_lamp_need_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>186wcmq</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Christmas nails have entered the chat 😍❄️✨</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186wcmq</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>186vpj7</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Purple and Blue🥰</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186vpj7</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>186vhzu</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>❤️❤️❤️</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t7lusgxqrb3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>186v40k</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Birthday Nails 😊</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0iikfjbvob3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>186uu4s</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>My first Christmas set using Mooncat polish! 🎄</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186uu4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>186ue55</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>First time doing skinny straight across French</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0am0dzmjb3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>186tt30</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Birthday nails ❄️ 💎</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bc8dopgefb3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>186tqvl</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>🩵My Xmas nails 🩵</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186tqvl</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>186tbul</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Burberry 🤎 my first time trying coffin and I think I like it!</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2hz7dtbubb3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>186t5a4</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>I'm so happy I got back into doing my nails, I've missed doing holiday themes. (':</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186t5a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>186rz3q</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Heard ya’ll like naked naturals</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5j8yljp1b3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>186rp70</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>I've been growing out my nails for three months ...</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/967k4ykjza3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>186rhhe</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>walgreens press ons can be so pretty</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfi67lmxxa3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>186r4je</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>A beary cute design on gelx!</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71e8xlx7va3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>186qxm5</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>My red nails</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/czdz2ckpta3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>186q99e</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Just a gloss on my natural nails</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzfrd059oa3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>186q1zw</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>will I be able to grow my natural nails out if I remove the acrylic?</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/186q1zw/will_i_be_able_to_grow_my_natural_nails_out_if_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>186pnkv</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Re-doing coffin nails?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/186pnkv/redoing_coffin_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>186ox3e</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Neonail LED Lamp</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/186ox3e/neonail_led_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>186obug</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Press on nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nq4drr4q6a3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>186nvah</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Soft Gel Tips Newbie</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/186nvah/soft_gel_tips_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>186nhb0</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Practicing xmas nail (gel x tips, gel builder, 5 hours down the drain, did only 4 nails 🤣)</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186nhb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>186l8zz</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Diy</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186l8zz</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>187da1b</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Let's talk about those "Reds"....show me which reds you're wearing for Christmas! I wanna see..... 🤗</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/187da1b/lets_talk_about_those_redsshow_me_which_reds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>187cf6a</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Tried Christmas nails. Not sure what I did wrong.</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187cf6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>187bbv6</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>💝✨️Kawaii Vibez✨️💝</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187bbv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1879zyt</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Anyone else have a problematic finger?</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1879zyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>18794gx</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>My fav red</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/snhtvt2gre3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1878233</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Mixed new colors using my de-stash pile!</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1878233</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1877sr8</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Can I apply DND gel on top of Kokoist builder gel?</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1877sr8/can_i_apply_dnd_gel_on_top_of_kokoist_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1877idu</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Obsessed with these Kiss press ons</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1877idu</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1877fiq</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>First Polish Pickup order arrived smashed</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdbg00vpce3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1875xxs</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Death Valley Nails “Jo-Ann’s Red”</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpi0sl8j0e3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1875v40</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Reminds me of a pretty museum floor</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1875v40</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1875rtf</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Did I do it right?</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1875rtf/did_i_do_it_right/</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1875lo8</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Zoya Sansa with Seche Vite Quick Dry topcoat. Hard to show the color - it's a bronzey purplish sparkly shade.</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upzte3rexd3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1874rtf</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Ether Dragon featuring kitty nose boop!</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vk7tif1rqd3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1874ri9</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Excitement to despair in one day</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1874ri9</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1874ddo</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Mario &amp; Sonic</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1874ddo</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1872oqm</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>The battalion is lost...</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8icscgead3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1871euf</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Hunt matching my moonstone perfectly !😍🫶🏻</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1871euf</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>187194l</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>2 untrieds and an old favorite</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187194l</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1870qxm</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Advice on growing out cuticles</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1870qxm/advice_on_growing_out_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1870bdv</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Accidentally seasonally-appropriate</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1870bdv</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1870b6r</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>It's giving a glam swamp</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kj6e3j5csc3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>186zrcp</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Jelly + Star Glitter</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186zrcp</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>186zjvj</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>I gave in. House of Hades + Disco Dust Taco</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186zjvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>186z47k</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Love Jellies</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blhyx0x6jc3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>186z0wi</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Thank you to the person who posted about the Zoya sale a few weeks ago!</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186z0wi</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>186ycf3</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>GASP. I love it</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eczsy0z3dc3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>186yahv</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Essie gel couture in bodice goddess</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d1x78eiocc3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>186y7sa</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>How would you rate this cuticle job?</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186y7sa</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>186xl7i</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Birthday nails</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eej9zlt77c3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>186wslg</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Ether Dragon</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zccdnkrn0c3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>186wfww</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>First Festive Manicure</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jsiboylnyb3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>186w86k</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>🌟 Magical Jelly Sandwich 🌟</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186w86k</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>186w4r2</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Glitter Toppers You've Tried</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/186w4r2/glitter_toppers_youve_tried/</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>186w13x</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Looking for a dupe for EDK Mahalo or something similar.</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/186w13x/looking_for_a_dupe_for_edk_mahalo_or_something/</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>186vzc0</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>LynBDesigns Alexandrite ✨️</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186vzc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>186uikq</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Where can I can purchase opi big apple red gel not as a beauty professional?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/186uikq/where_can_i_can_purchase_opi_big_apple_red_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>186vgau</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>SYS - Weekly Challenge #3 - I’m a professional.</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186vgau</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>186s6it</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>New here!!</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5v7i38n83b3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>186urq0</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Broke my nail so all of them have to be short now</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186urq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>186upnr</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>I love this magical green shimmer! ✨</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/khvewynzlb3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>186uki5</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Recs for YouTubers with warm undertones?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/186uki5/recs_for_youtubers_with_warm_undertones/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>186tcfo</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Any tips for removing ORLY Builder in a Bottle?</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/186tcfo/any_tips_for_removing_orly_builder_in_a_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>186tau3</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>How can I prevent my edges from looking rough?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ntawphynbb3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>186ta4b</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Purple Zoya Skittle</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186ta4b</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>186s6m4</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Christmas!</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a2q3x8993b3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>186qq5h</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Storage for Mooncat Polishes</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/186qq5h/storage_for_mooncat_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>186qdwp</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>My favorite ILNP collection + reflective taco</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186qdwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>186qcmz</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Question: painting damaged nails?</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/186qcmz/question_painting_damaged_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>186ploa</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>How do you organize?</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsq8jmhria3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>186pjwk</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Started rock climbing this year, trying to get back into liking my nails even though I have to keep them short now 🧗💅</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186pjwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>186n6cg</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Is leaving a few mm of space on the sides of the nail strange? I've always done it but a girl told me it's bad. I usually do it because it optically lengthens the length</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blhn56jau93c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>186l62d</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Death Valley Nails - Cobalt Blue Pencil 💙</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zq1rej0f593c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>186l2tc</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>MY POLISH HAS LASTED 36 HOURS</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/28cwfwu9493c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>187c764</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>My first time doing nail art. Any suggestions?</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ueug01rlf3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1878unw</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Late fall | Nails matte vs shiney (excuse the non-oil-cuticles)</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1878unw</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1878jul</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Penguins! ❤️</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1878jul</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1878gsd</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>I’m having trouble getting onboard with holiday nails bc I’m really into cats 😂</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y4ihhm3hle3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1876f4l</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Acrylics still be queen imo</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1876f4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1870ccl</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>My new holiday/Hanukkah nails (painted by Coated Fort Lee)</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5m38o5lsc3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>186xxvi</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Butterfly nails..</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.redgifs.com/watch/nauticalrevolvingnorthernspottedowl</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>186vxxq</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Holiday nails</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zubsv250vb3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>186quex</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>New set ✨</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186quex</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>186mzia</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Are mermaid nails still trending?</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/186mzia</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Dec  1 08:08:21 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_03.xlsx
+++ b/data/2023_12_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C732"/>
+  <dimension ref="A1:C885"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12877,6 +12877,2607 @@
         </is>
       </c>
     </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1885e7e</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>I want to buy my wife a nail kit similar to the one she used in Japan, what do I need?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1885e7e/i_want_to_buy_my_wife_a_nail_kit_similar_to_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1880fyi</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Should I ask for these to be fixed?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1880fyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1885mek</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>🩷Matching set🩷</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udbcfbwetm3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>187xj3w</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Did my birthdays nails inspired by Charlotteherberts2 on TikTok</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65994dh4sk3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1885ir2</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Nail shape!</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1885ir2</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>18858z9</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Help with taking off acrylics that I got recently.</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/18858z9/help_with_taking_off_acrylics_that_i_got_recently/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1884ae4</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Red Chrome French Tips 💋</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o47r5ulafm3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1883wm6</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Nude-ish Claws</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1883wm6</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1883vty</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>A little Christmas set I did on my broken crappy nails 🎄</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1883vty</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1882qbp</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>rose+gold set</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1882qbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>18826wu</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Love this color combo!</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27729azevl3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>18824cv</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Rubber base is my new BFF</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0naflnqul3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1881z6a</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>I love this color</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ida5bbaetl3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1881quq</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Icicles ❄ temp changing </t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bttbwcr4rl3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1881ph8</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>My mom’s nails that she gets done at her local salon</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1881ph8</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1880e4y</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzoqmfclfl3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1880dxz</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Octopus for Turks Vacation</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iopqv6qjfl3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>187zyz2</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Tips for anxiety nail pickers/biters</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/187zyz2/tips_for_anxiety_nail_pickersbiters/</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>187zj5a</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>I’ve always hated my nail beds but I’ve been growing out my nails since giving up dip powder about 4 months ago.</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vusj24t88l3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>187zfhm</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>How to fix nails that are broken past the quick?</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dnz9t7f7l3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>187z8mh</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Gold Chrome</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9841kmv5l3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>187yrc9</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>These Etsy press ons did not disappoint 🖤</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klk3wq2x1l3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>187xy1m</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Do yall think these are cute ?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrfj9rqhvk3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>187xvbl</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>LMAOO</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/187xvbl/lmaoo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>187xk1q</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Christmas Nails🎄⛄️</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1f0zh6csk3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>187x7xq</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>probably my coolest set yet</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redgifs.com/i/lightslategraytaninvisiblerail.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>187wxeg</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Vero Beach, FL Nail salon Recommendations?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/187wxeg/vero_beach_fl_nail_salon_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>187wqoc</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Claws</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbjh841wlk3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>187whfr</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Freshly set, love grey</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9xfoh7yjk3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>187w9ec</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>I love my natural nails</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187w9ec</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>187w1tg</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>In love with the simple shimmer and accent nail!</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ap80wpcngk3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>187vij0</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Gel polish colors similar to Kylie pink and camation pink by beetles ?</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxc0fsyqck3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>187v70j</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>I keep going back to this shade, I can’t get enough🩷 Mooncat’s Velvet Rose 🌸</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187v70j</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>187v51a</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Rate my beginner gel nails</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mv34wqfy9k3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>187v486</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0ivmw8s9k3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>187v27k</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>first time tips and it's so cute i love it!!🥰</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187v27k</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>187v24x</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9g4y0tc9k3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>187txwo</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Shape suggestions?</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187txwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>187tnem</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Coquette black and white</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ry2juin1zj3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>187tk1p</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>as a nail tech it’s hard to find time to do my own nails but i managed! bows handpainted by me 🎀</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ngn0xv7cyj3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>187t37g</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>It's officially Christmas season! 🎄</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8xkjq91vj3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>187sx1n</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Best rubber base to use without buffing?</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/187sx1n/best_rubber_base_to_use_without_buffing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>187skpw</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Long or short nails for Christmas?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/187skpw/long_or_short_nails_for_christmas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>187ro19</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Almost didn't do my right hand cause I was tired 😂</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187ro19</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>187sa85</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Chrome green!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187sa85</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>187ryeu</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>CowPrint 🐄🐮</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187ryeu</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>187rh10</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>If I use non-acetone to take polish off, can I technically paint them once a week?</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/187rh10/if_i_use_nonacetone_to_take_polish_off_can_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>187r6lq</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>How did I do for my first set of gels on my friend. Who had a lot of wine? Looking for honesty</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0e3n9upgj3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>187qgrh</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Graduation nails🎊 Receiving my BFA next week.</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20l2lpsbbj3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>187pzg2</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>my bf and i got our nails done again :)</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upsd2tbm7j3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>187p7hk</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Winter nails ❄️</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drkvs60q1j3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>187owst</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>My first wintry nails of the season!</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atbmqeuezi3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>187oqwi</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Decided to go with a color other than chrome black....</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xk6ssi99yi3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>187n5xs</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Went back to my usual nail salon and I couldn’t be happier with the results</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jc3x5ii7mi3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>187n1tz</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Favorite UV gel polish brands?</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/187n1tz/favorite_uv_gel_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>187mwan</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>grabba’s</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avbmmj85ki3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>187efjp</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>I can’t wear nails for work, what’s a non-permanent solution for wearing nails?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/187efjp/i_cant_wear_nails_for_work_whats_a_nonpermanent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>187mjns</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>nails I did for a client! was $35 :)</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4mhzjqkhi3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>187m5rs</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>cool frenchies 🧊</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187m5rs</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>187m0gz</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Christmas set I made</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187m0gz</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>187l619</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Edge of nail grows in broken?</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187l619</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>187kilh</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>My new nails!</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kw1148g12i3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>187khto</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>EVERYTIME i do my nails there are bumps or bubbles</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/blcjsgjv1i3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>187k24s</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Love my simple Christmas nails ✨🎄</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05n6vbifyh3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>187k0yf</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Almost holiday nails 🎄❤️</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187k0yf</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>187jw9i</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>When you’re walking home and casually pose with a tree 😅</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yeo0tc85xh3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>187jbuo</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Is Venalisa a good brand?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/187jbuo/is_venalisa_a_good_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>187izsu</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Boring nails of the week 💅</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8gk1xmssph3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>187iuz1</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Finally got the hang of cat eye/velvet nails!</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hqp43i4moh3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>187hygl</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>First time using builder gel on my natural nails</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y13c6cojgh3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>187h489</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Feeling a little christmassy, but not ready to give up autumn nails</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187h489</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>187gk8n</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>My new nails, so shiny ✨</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187gk8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>187fsxu</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Growing out my naked nails</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187fsxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>187femr</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Is this nail worth 100$</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187femr</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>187fclp</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>I tried a new nail tech this week</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zc36ybwwng3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>187f6dy</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Favourite set I’ve done so far✨</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6438mnvolg3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>187e846</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>what is your opinion on different coloured polish on each hand ?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/187e846/what_is_your_opinion_on_different_coloured_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>187duid</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Christmas Nails ❤️💅🏻</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4rgnlu65g3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1886fa2</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>About to give up on diy gel nails - please help!</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1886fa2</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>187vhec</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Color recommendation request to match engagement ring</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/187vhec/color_recommendation_request_to_match_engagement/</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>18857g7</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Thank you all for potentially saving me from a gel allergy 🙏</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18857g7/thank_you_all_for_potentially_saving_me_from_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>18852f7</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Finally doing nail art after 14 years of being a professional chef</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4xtkq69nm3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1884h4a</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Advent calendar reveals?</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1884h4a/advent_calendar_reveals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>18844g8</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Pistachio shorties 💚💅</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/re7l03oqdm3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>18820h6</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Does anyone have a swatch of Mooncat’s My Bugs! my Bugs! Vs their Warp Zone?</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18820h6/does_anyone_have_a_swatch_of_mooncats_my_bugs_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1881z17</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Joined the HOH bandwagon</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1881z17</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1881wy3</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Jet Setter 🤩</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ryzd7estsl3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1881kf0</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Very proud of the overall shape of these!</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkznbmzrpl3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1881eiw</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>They ain’t perfect, but their mine</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1881eiw</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1880sxc</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Blue shorties! Perfect color for a rainy day.</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1vj9msp2jl3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>188019k</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Cirque’s Ethel</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1l8quficl3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>187z5z9</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>How do I organize my 229+ polishes? 😭</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/187z5z9/how_do_i_organize_my_229_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>187z5e0</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Holiday party in a bottle</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187z5e0</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>187y3zv</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Jumbo Magnets</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/187y3zv/jumbo_magnets/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>187xxz9</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>First thermal, I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187xxz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>187xibq</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Essie’s Shine of The Times (dupe) GEL dupe?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/187xibq/essies_shine_of_the_times_dupe_gel_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>187xp87</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>ORLY November Fog ✨️</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187xp87</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>187u5mc</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>The Best of the Best</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/187u5mc/the_best_of_the_best/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>187x5q6</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>I'll never say no to a vampy shimmer</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187x5q6</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>187wyq8</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>2 Months of Nail Growth!</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1purqwbnnk3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>187v7xu</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>I keep going back to this shade, I can’t get enough🩷 Mooncat’s Velvet Rose 🌸</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187v7xu</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>187v1oz</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Nails super thin and peeling</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9wt0nt89k3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>187uuvl</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>My winter manicure</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65hfe0rt7k3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>187up65</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>My attempt at an Ethereal Cloud Latte dupe</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rwzs3om6k3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>187uek6</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Painted for the first time in ages</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jix7794h4k3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>187u64b</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Ether Dragon has my heart 🐉💜</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187u64b</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>187tnxc</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>🦄 + 🧜‍♀️ = 💅</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187tnxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>187tl2d</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>always hard to find time to do my own nails cause i’m busy making everyone else’s nails cute! handpainted bows by me! 🎀 (__kmnails)</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yml8lfzjyj3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>187tf5l</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>“Girl Dragon” by Phoenix (November PPU) and “Cameo” by ILNP</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187tf5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>187splf</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Holo Taco Disco Dust on bare nails</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/187splf/holo_taco_disco_dust_on_bare_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>187rqts</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Mooncat - Pangea</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187rqts</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>187ri2q</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Thinned out / Rehydrated Holo Taco Rainbow Snow makes a super sparkly and easy to use topper 💎</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqn75pl4jj3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>187ri04</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>How to prevent diffusion in magnetic *non gel* polish?</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4v87xz3jj3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>187rh4e</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>color similar to sally hansen tenacious ruby (circa 2012-2013ish?)</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187rh4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>187r5su</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Dark Rainbow Fun</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ayqppyjgj3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>187qkt7</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>House of Hades in the sunshine 🤩</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pda2auj6cj3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>187po3h</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Quick Dry polish tips</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/187po3h/quick_dry_polish_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>187pmh6</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>My phone camera can barely cope ✨</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187pmh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>187p8yc</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>💕Cotton Ice💙 because my drive way is covered in ice 🙃</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187p8yc</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>187p6zy</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Warp Zone 🛸💚 plus my first attempt at a French mani</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187p6zy</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>187ovcf</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Friendly reminder for neurospicy goblins like myself - put stuff up after nails are finished</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/id52d264zi3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>187oq5z</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Desperately trying to keep my thumbnail from breaking any further 😫</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187oq5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>187o428</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>I love mixing gloss and matte with nail art.</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187o428</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>187o2zx</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Little fly agarics</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hkv3b96ati3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>187nti7</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Is it just me or does Midsummer's Dream look like chrome powder?</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gild1va8ri3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>187mdn9</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>nail care</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/187mdn9/nail_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>187mknl</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Grace by ILNP in and out of sunlight 💖</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/li4qpbdshi3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>187mh02</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Getting back into nails after becoming disabled</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sesenak0hi3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>187met0</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>How long does your typical lacquer mani last?</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187met0</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>187lvtq</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Man-e Pedi? Too weird?</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ua272lpoci3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>187lt2h</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Obsessed over Large Particle shifty polishes!</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187lt2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>187ls55</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Behold the shine!</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwjr75wobi3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>187lqfy</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Reorganized my polishes and now I have room for more!</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6nqaauzgbi3c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>187lh4y</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>I love green, so 5 green polishes it is then 💚</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0xk08mi9i3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>187ldto</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Hack: use kitchen roll to take off your polish</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/187ldto/hack_use_kitchen_roll_to_take_off_your_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>187lb5r</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Cirque Colors is re-releasing Coronation tomorrow</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/187lb5r/cirque_colors_is_rereleasing_coronation_tomorrow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>187kjsl</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Sovereign Teen Spirit</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0nyw3z92i3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>187jtp9</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquer - Snow Queen</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187jtp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>187jpsb</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>{PR} The Nightlife Collection by ILNP 😍</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zjbldspvh3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>187iodo</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>"Looks like 'Old Money' " --My partner</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vupsqtc1nh3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>187ibzl</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>both disappointed and impressed with my first non-drugstore purchase…</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187ibzl</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>187h1a0</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Feeling a little christmassy, but not ready to give up autumn nails</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187h1a0</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>187et7t</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>The absolute chokehold magnetic nails have on me lately</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w0jkqmj3hg3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>187elwk</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>I can't live without magnetics</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jlw1jwpleg3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>187dkdd</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Keeping warm</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187dkdd</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>187dk33</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Does everybody here have beautiful hands?!?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/187dk33/does_everybody_here_have_beautiful_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1881qur</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Icicles ❄ temp changing </t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vjdwknevql3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>187zy91</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Holiday bows</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187zy91</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>187udgn</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Black Magic</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187udgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>187sryk</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Black &amp; Gold Present Nails by me</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iomslnznsj3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>187p3c0</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Christmas vibes</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187p3c0</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>187kqps</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>🩷 tweed nails</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h9j60atq3i3c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>187h8wz</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Feeling a little christmassy, but not ready to give up autumn nails</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/187h8wz</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Dec  2 08:07:10 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_03.xlsx
+++ b/data/2023_12_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C885"/>
+  <dimension ref="A1:C1046"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15478,6 +15478,2743 @@
         </is>
       </c>
     </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>188w165</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Not the intended look but like the end result nonetheless</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9u3qket0ct3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>188tnao</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>How much is too much for gel manicures?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/188tnao/how_much_is_too_much_for_gel_manicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>188t811</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>New Nails! Holo to heal the soul 🥺</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/c0mhuociks3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>188xvwj</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Tried nail art. Took like 5 hours to do but was ☺️ Aha</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188xvwj</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>188lxml</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>I've never really done nails like this before did they turn out okay?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188lxml</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>188wqs8</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Sad because ive gotta keep my nails short(er) cause work fucks them up, at least its satisfying to file the wonkiness</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6p21x2gdjt3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>188wmi5</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>purple winter nails</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibessyn6it3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>188wm4k</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Did these while feeling silly 🌈🌈🦄</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6besiou2it3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>188wm07</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Christmas nail stickers ✨️ 🎅🦌 I'm still learning, so be kind. I'm gonna add red crystals on the holly on my pinky when they come in the mail.</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188wm07</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>188w6yd</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>My DIY Christmas set! 🧑🏻‍🎄</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5snkb2mndt3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>188w148</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Got my nails done! 36$ in Vietnam.</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188w148</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>188uw6l</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Christmas nails ❄</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188uw6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>188ulnm</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>My first time with red nails</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188ulnm</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>188ubcq</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>I have one nail that always snags terribly if i grow my nails longer. Is it fine to put gel over the snag? I just don't want to make it worse.</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjyfjmfous3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>188u9c7</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Winter nails</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188u9c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>188sgld</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>I have literally no idea how to take cute pictures of my nails 😭</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188sgld</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>188s5n7</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>what's your favorite gel cat eye polish?</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/188s5n7/whats_your_favorite_gel_cat_eye_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>188rvhw</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>French Mani</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/188rvhw/french_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>188rd9n</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Soooo happy with my new nail tech!</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgf2s2g14s3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>188r03a</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8r6rbix0s3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>188qz7b</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Go Dawgs, sic ‘em (3rd set ever)</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aj71qjiq0s3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>188pr92</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Dip Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188pr92</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>188p6y2</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>I tried getting acrylics for the first time in years and I was disappointed</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188p6y2</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>188p2ry</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>How can I improve my nail?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekmj7kx0lr3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>188p25i</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>love these Kiss Impress Nails😍</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3yikxibwkr3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>188odt2</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Struggling with nail art</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/188odt2/struggling_with_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>188o2nr</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>KC Nail Lovers- Where do you go?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/188o2nr/kc_nail_lovers_where_do_you_go/</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>188nydd</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Pink glitter nails💕! I absolutely love how these turned out! (I know they’re not perfect but I’m still new to this)</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vs6gbtfybr3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>188nqt3</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>new nails, did them myself!</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c9we4sybar3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>188n45r</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Chrome for Christmas 💚</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5emue3j5r3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>188mk5q</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Revlon Red Nails</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188mk5q</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>188mgxs</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>My nail art brushes finally came so here’s my first attempt and I’m in love🥰</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2msx9n9i0r3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>188m244</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Christmas ornament set 🎄⭐️</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188m244</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>188m0ax</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Newest DIY set :)</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pem94a9ywq3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>188m00g</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>No place like chrome for the holidays 🎄</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q161qiowwq3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>188lu7f</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Wintery cherries</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188lu7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>188l453</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Sticky bottles</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/188l453/sticky_bottles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>188kzig</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Best My Nails Have Looked</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/379vb201pq3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>188kuuq</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>I bought these cute little Christmas stickers, wondering what base colour I should do?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188kuuq</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>188klew</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>My first gel manicure</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188klew</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>188juwg</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Got my nails done yesterday and I’m in love</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5d0vhax3gq3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>188jomc</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Newbie and probably a dumb question</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/188jomc/newbie_and_probably_a_dumb_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>188jfzi</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Gel builder set done by my mum :)</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qne2x46vcq3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>188janl</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Did blush nails again, but added some multichrome flakes eyeshadow topper</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xou372mpbq3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>188j385</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>How to fix my destroyed nails</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/188j385/how_to_fix_my_destroyed_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>188ixf5</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Ice world ❄️</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188ixf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>188ikvm</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Some of the years looks by my awesome nail tech!</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188ikvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>188ii1e</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>natural, polish only 💖</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xta7wa9o5q3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>188i8l1</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Getting my nails done later today for getting married this weekend.</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188i8l1</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>188hwp6</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>matching donnie darko nails on me &amp; my bf</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ew3srli61q3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>188htic</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Hailey Bieber almond nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ck4maih0q3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>188hoke</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>what do we think of the winter duck nails</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gc8yijdgzp3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>188hbya</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Soft pink nail art with some gold details ✨️💕</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188hbya</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>188h2y1</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>My Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nzi5ajaxup3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>188gltf</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Unfortunately Disappointed 😔 - Rant</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/188gltf/unfortunately_disappointed_rant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>188gk3g</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>has biab nails weaken my natural nails?</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188gk3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>188fvn8</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Nail shape opinion?</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1e45p7qlp3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>188d6b4</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Nail Newbie — Need Advice!</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/188d6b4/nail_newbie_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>188g9io</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Loving this blue! 💙</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsguxu0rop3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>188g6f5</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>✨Intergalactic Invasion✨</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8t1s4xo2op3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>188g63l</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>December means Christmas nails</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azgchsh0op3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>188g1k6</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Latest manicure</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eeukgtb1np3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>188fojp</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>My dark nails</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3x410t27kp3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>188eo7g</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Tried a builder gel for the first time.</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188eo7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>188eer7</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>So adorable blue nails</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188eer7</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>188e8wt</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Gave myself some wintery nails. They're 3 weeks old now, but better late than never!</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u22kgt3o8p3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>188e3om</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Fun nail product recommendation for girlfriend</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/188e3om/fun_nail_product_recommendation_for_girlfriend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>188e10l</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Picked a new salon, was $80 too much?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188e10l</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>188dsbh</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Trying to grow nails longer, but this one keeps bending. Is there anything I can do to make it grow straight?</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188dsbh</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>188djgx</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>My Christmas Nail Set</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6x79ktzx3p3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>188de7r</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>CND Strengthener Rxx or RescueRxx??</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/188de7r/cnd_strengthener_rxx_or_rescuerxx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>188d3e2</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>My nails</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188d3e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>188cbmt</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>What kind of nails/nail beds are these? Is there any name? I have never bitten my nails. I have seen nailbiters with such small nails and they seem get long nail beds when they stop biting.</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3rlip80juo3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>188cbbi</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>loveeee my new set</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188cbbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>188bkt1</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>A series of unfortunate events...</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kj9bqyj4oo3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>188bhzx</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>What do you think about the colour for this summer?</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mxlc7aeno3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>188bhe6</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Starry twilight December nails!</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188bhe6</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>188bhd1</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>I dig it 🤙</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clluddn8no3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>188aomv</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>It’s the season ladies ✨</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzxig9rqfo3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>188aher</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>DIY Christmas Nails 💙 The last time I had my nails done in blue was when I found out my baby's gender, he's turning 1 in a couple days.</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3165h0rdo3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1886o41</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>obsessed with my nails!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h58t7dss5n3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>188ycto</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Suggestions Pink &amp; Green!</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188ycto/suggestions_pink_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>188x83n</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Starrily Jellies Sandwich</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uxc6j2pkot3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>188wxlc</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Something similar to Zoyah’s Maisie?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188wxlc/something_similar_to_zoyahs_maisie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>188wuub</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>is it morally acceptable to do my nails in public…</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188wuub/is_it_morally_acceptable_to_do_my_nails_in_public/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>188wuqj</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Death Valley Nails question</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188wuqj/death_valley_nails_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>188wo8p</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>This is the most risky thing I've done so far. Gel with stickers. I'm trying to do better with shaping my nails. I will try free handing next.</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188wo8p</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>188w4h6</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188w4h6/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>188w0ay</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Dupe for Orly coconut milk?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188w0ay/dupe_for_orly_coconut_milk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>188vt00</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Girl Dragon from Phoenix Indie Polish</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188vt00</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>188vnc0</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Happy December! (My fave month of the year ☃️🎄)</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188vnc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>188v7wn</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Revlon Divine</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188v7wn</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>188ua30</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>What kind of silly things do you do on mani nights to deal with not having fingers?</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9mj76gcus3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>188u3w2</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Good or bad gift for a mom ? ( It's nail polish related I swear )</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188u3w2/good_or_bad_gift_for_a_mom_its_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>188u1dc</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Cute with a single coat</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188u1dc</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>188twm3</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>I do love a cloudy day.</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188twm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>188tvcd</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Yet another no-gel chrome mani 🩷💜</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188tvcd</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>188t48o</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Christmas inspired nails</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188t48o</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>188rlbt</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Trying to make the best of my shorties after damaging them</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188rlbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>188r7qi</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Newbie Learning at 40+</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188r7qi</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>188r70v</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Frosty blue for the first day of December</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwpbo9fk2s3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>188r0o8</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>If I’m really careful to not get Beetles nail polish on my skin, will I be ok??</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188r0o8/if_im_really_careful_to_not_get_beetles_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>188qndu</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>You think you've seen them all but then...</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjj9qmlzxr3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>188qmf5</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Lehabah🌙 🌇 🔥</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188qmf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>188qfv7</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Matching undertones</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggz3ir08wr3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>188q7ng</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Xmas nails at home</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188q7ng</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>188q06c</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Ordered nail polish from mooncat and received an empty box, has this happened to anyone else?</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cocdf5vksr3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>188pjyo</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>One nail painted with Cupcake Polish Ghoul Friend</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckjnu0vtor3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>188p9wp</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Builder gel lifting</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188p9wp/builder_gel_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>188p7lc</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Which frequently recommended “true reds” do you NOT consider to be a true red?</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188p7lc/which_frequently_recommended_true_reds_do_you_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>188ow7i</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Late goblins &amp; ghoulies appreciation post ❤️</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188ow7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>188or4r</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Dupe for Sassy Cats Lacquer: Sugarcoat Everything?</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188or4r/dupe_for_sassy_cats_lacquer_sugarcoat_everything/</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>188nqqj</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>beginner skittle</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188nqqj/beginner_skittle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>188mu3v</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Need help with Oh Splat!</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bij4fjd3r3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>188mq9x</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Help! My nails are so flimsy! Looking for recs</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188mq9x/help_my_nails_are_so_flimsy_looking_for_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>188mmfi</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>My nail art brushes finally came🥰</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2k50c9un1r3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>188m9fw</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>I did a thing y'all!</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9n89ejwyq3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>188m2qa</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>My first set of press ons!</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ck1fmfshxq3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>188ltmp</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Color Club We’ll Never Be Royals</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188ltmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>188ll0k</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Tinsel Swirls🌀🌀</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6j1x61rtq3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>188l5s9</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Day 1 of Nailvas</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljg2cqseqq3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>188kle7</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Nails for wedding dress pickup!</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188kle7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>188jz8k</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Taco Took a Drive</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9j5rpl43hq3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>188jrw8</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Mooncat Limited editions - how "limited" is limited?</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188jrw8/mooncat_limited_editions_how_limited_is_limited/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>188jfam</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Cock-a-doodle-doom but make her dark ✨</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188jfam</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>188jexm</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Christmas Nails Attempt</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3r8h9rmcq3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>188j1ma</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Ice world ❄️</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188j1ma</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>188j178</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>She’s pretty, but…</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5huyqxn9q3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>188ir20</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>How come nail polish only comes in glass bottles but polish remover and polish thinner is available in plastic bottles?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ns8ouikj7q3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>188ills</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>I love OPI's formula but the colors are so boring</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188ills/i_love_opis_formula_but_the_colors_are_so_boring/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>188il2y</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Cozy Turmeric vibe - Essie in shade Buzz-worthy Bash</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lwb8kdb6q3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>188ikas</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>First Holiday set of '23 🎄</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jb4p26l56q3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>188humq</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>H&amp;M - Devon Violet + China Glaze - Fairy Dust</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188humq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>188hsvy</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>This blogger compared the newest Cirque Coronation release to previous versions</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188hsvy/this_blogger_compared_the_newest_cirque/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>188h8w4</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>It's been six months since I got married, but I'm still obsessed with my wedding nails</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188h8w4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>188h5ra</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Coffee Teddy Bear Press Ons</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188h5ra</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>188grjk</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>A little vampy, a little festive</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188grjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>188g9ha</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Dupe for Ethereal Lacquer Hourglass?</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188g9ha/dupe_for_ethereal_lacquer_hourglass/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>188fzol</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>I have over 100 polishes now and bought my first Helmer</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/898hi4xlmp3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>188fy1w</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Smile line taken literally</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58yd25p8mp3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>188fa67</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>How do you avoid getting overwhelmed?</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188fa67/how_do_you_avoid_getting_overwhelmed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>188eodn</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Favorite non-sparkly color shifting chromes?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5z7zfxljcp3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>188edff</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Is it right for the re-release of Cirque’s Coronation to be a different base color, shimmer, and holo pigment than the original (and 2017 re-release)?</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188edff</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>188e1gl</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>First Christmassy set this year! Happy December</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78e1ggel7p3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>188djly</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Not to be an enabler or anything… but yes, you do need Coronation by Cirque Colors 👑</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188djly</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>188cvn7</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>This shift is unreal!</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188cvn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>188c7j8</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>What is your favorite top coat?</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188c7j8/what_is_your_favorite_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>188c5n5</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>What kind of nails/nail beds are these? Is there any name? I have never bitten my nails. I have seen nailbiters with such small nails and they seem get long nail beds when they stop biting.</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4ofgzkrso3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>188bl4w</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Black Cherry Chutney - OPI</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/ComQt6W</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>188bfe4</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Allergy question</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/188bfe4/allergy_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1889b5a</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>My collection has grown in 10 months 😄</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1889b5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>18897bf</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>PPU Monthly Megathread</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18897bf/ppu_monthly_megathread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>188w9vy</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>A few nail sets I’ve done on myself</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188w9vy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>188r9wg</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6lz7vn883s3c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>188o5td</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Some eyeshadow nails</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188o5td</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>188nnq8</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188nnq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>188m0hx</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>What to do on my thumb?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpm3t4k0xq3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>188k7mr</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188k7mr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>188fmb3</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Finally! Holographic aurora nails- wich one do you like more?</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188fmb3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>188erh2</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Christmas designs diy</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188erh2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>188cqvx</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Two nail sets i did for myself!</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/188cqvx</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Dec  3 08:07:22 UTC 2023
</commit_message>
<xml_diff>
--- a/data/2023_12_03.xlsx
+++ b/data/2023_12_03.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1046"/>
+  <dimension ref="A1:C1191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18215,6 +18215,2471 @@
         </is>
       </c>
     </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>189oqrt</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Winter nails ❄️ 💅</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189oqrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>189opt8</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Most recent gel manicure.</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzd4cfxnc14c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>189ol47</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>How to properly care for natural nails</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/189ol47/how_to_properly_care_for_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>189nef1</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Todays nails!</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ghxefndw04c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>189ms68</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Christmas Nails 🎄♥️❄️</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5ogtzyr9p04c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>189mhod</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Wanna help me narrow em down?</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9k3bipwzl04c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>189m2sp</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Best easy DIY manicure for new mom</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/189m2sp/best_easy_diy_manicure_for_new_mom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>189kwau</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Y’all I need help! Is it normal for nail techs to do a couple layers of clear dip powder then use gel to add color?</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8lmtepej504c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>189kexg</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my mom's nails! </t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nx8hqkjx004c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>189jvi1</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>My new nails have been cat approved</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189jvi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>189jrat</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Flash Gel</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189jrat</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>189jpa7</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Hello kitty nail set I did!</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zv9y0jttz3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>189jmpb</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>My natural nails painted with Dazzle Dry</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihudzfc3tz3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>189jj0u</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>My real nails painted with OPI Dutch Tulips 🌷</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atge8aj1sz3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>189jirr</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Hotel nails!</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9tnld21zrz3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>189je58</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Ive made my first Chtistmas nails!</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189je58</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>189iuwm</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Cute green set I did today</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hgxgsvalz3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>189iqmd</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>🌿💨💖</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189iqmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>189io97</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>❄️ Snowflake French nails ❄️</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/idjue5lfjz3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>189img2</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/189img2/what_am_i_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>189iju2</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>My holiday nails!l</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmamifr7iz3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>189ijl5</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Christmas nail set I made</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvkr8xi5iz3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>189idn4</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Holiday Nails</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77c3q3fjgz3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>189i88p</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>In love with my Hanukkah nails🕎⭐️</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79cu47b0fz3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>189i5tl</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>My first stiletto set ❤️</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189i5tl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>189i0a3</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>First set of Christmas nails 🤩</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ev268o1wcz3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>189hww1</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Girlfriend paid $40 for these. What do you all think?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdocy1pybz3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>189hneu</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Winter Themed</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgubjj3f9z3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>189hkwu</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Just a fill 🫶🏼</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6luydcr8z3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>189hhq2</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Glitter ombré with Have a Holographic Christmas from Double Dipp’d</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dezixhy7z3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>189hfrp</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>First ever gel x</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35y6h3lf7z3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>189h3pd</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Obsessed with Chrome powders</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cecvmwe74z3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>189g4rm</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>I never get green, but this color was too good to pass up🎄</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/co0646cbvy3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>189g29r</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>My natural nails contribution =)</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i8fj52xouy3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>189fh51</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Finally bit the bullet and tried cat eye nails. I love them!</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yd2lpu7jpy3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>189f46p</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Was looking for a candy cane vibe; happy I got it</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189f46p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>189er3e</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Fresh gel nails</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asxe1vm9jy3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>189em94</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Nail broke and had to cut them short, but loving the glitter</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xb7meup2iy3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>189efqo</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Walking in a winter wonderland ❄️🎄</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bslqd3fggy3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>189e0c1</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Butterfly nails 🦋</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189e0c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>189dvj9</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189dvj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>189dhub</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Are these gel extensions too thick? What can I do?</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189dhub</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>189b969</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>I’m not sure what this shape is called, like rounded square? Does it look weird?</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189b969</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>189ag4h</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>new Christmas nails inspired by u/weirdemogirl</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189ag4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>189csgc</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189csgc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>189co4x</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Bing bang booya 🎉</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tuv8rq21y3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>189cdjy</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Press on Nails Rec?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/189cdjy/press_on_nails_rec/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>189bmci</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Merry Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ag0oxvh7sx3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>189av5r</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Tips for press ons??</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6l33vjvvlx3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>189aezn</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Gift for Niece who likes Gel-x?</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/189aezn/gift_for_niece_who_likes_gelx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>189a45d</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Christmas red</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/in496z5gfx3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1898yap</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>dreaming of a magnetic christmas 🎄</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ejj4maqn5x3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1898dg0</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Can I do anything about this growth on the sides, or do I have to leave it alone?</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfiscvuv0x3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1895tsw</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Little Debbie haunts me</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9hvamv8sew3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1898jjs</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Chrome snowflake nails ❄️</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lb1lxugb2x3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>188khuo</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>When / Where do you cut off damaged nails?</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/188khuo/when_where_do_you_cut_off_damaged_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1898f9l</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>holoooooooo</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6rmgiba1x3c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1897zcn</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Loving this INLP color!</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ofpdin8mxw3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1895l43</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Light Elegance JimmyGel not working?</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ltcpp1pcw3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>18965j3</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Koi Pond</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/18965j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1895zwg</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>did blue blush nails for winter ❄️</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exu6o2bbgw3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1895eqa</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Pinkmas nails 💖💖</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1895eqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1894pxe</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>My new nails . Love natural colors.</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rybmcrr4w3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1894ee1</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Nailfie Prop And Accessories</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1894ee1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>18945ey</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>My nails</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5tr9waifzv3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1893mk5</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Love my weird colours</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02uydvrguv3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1893gnj</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Newest Set</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wsb33hyssv3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1892z0c</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3890ybpnv3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1892awe</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Taking off gel getting ready for a new design</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rxe22w0gv3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>18929d5</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Ballerina red french ❤️</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ayfqcgrkfv3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1891iso</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Just applied some new press-ons. Was €3.49 too much? ;p</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b8zspdne6v3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>189178j</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Love this design</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyy9vbcq2v3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>188z3md</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Wintery nails for December!</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8q3cb8ajbu3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>189o0wj</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Simple</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/mAsV5DV</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>189nugu</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Just Playing with Bling Options</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iz8yvvmp114c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>189leun</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>She’s a stunner</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189leun</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>189kri1</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Best guess to closest polish color?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4ifx6q5404c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>189jryu</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>I gave in to the seasonal hype</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189jryu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>189jocx</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Essie “Off Tropic”</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189jocx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>189jgty</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Reflective polish never gets old. 😭🤩</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ybf11ewdrz3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>189imb8</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Little Christmas Trees</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189imb8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>189hyuc</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Another day, another chrome polish ✨</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/r91ephshcz3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>189hyds</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Lynb Alexandrite</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189hyds</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>189hciu</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Palestine press ons!</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q0z2wvrk6z3c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>189h9sc</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Which nail shape suits my hands better??</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189h9sc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>189h74b</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Clionadh Psilocybin velvet effect (various lighting)</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bhbdyih35z3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>189h0x8</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Struggling with nail peeling</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/189h0x8/struggling_with_nail_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>189gsbo</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Crushed Velvet 🎀💗😌</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189gsbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>189g57y</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>💅🏻 Storage box 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189g57y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>189fytv</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Favourite neutral: F.U.N Lacquer - Foggy</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189fytv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>189fpzi</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>ILNP Spiced Cider is my favorite color of the season</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189fpzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>189fm8c</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>My nails match the new stickers I’m making</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvc17lfqqy3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>189ff5y</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Barry Blue</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/heawzyn1py3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>189f10f</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t xml:space="preserve">We have Ether Dragon at home </t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/biwkxrcnly3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>189evs2</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Artemis Deathkiss</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189evs2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>189esu9</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Are these different? Lol</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zm4r0llojy3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>189ek44</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Antivenom Mooncat</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lxnq988jhy3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>189dtv1</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Swatching itched my brain</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/glwkicl3by3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>189dk1t</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>I Scream Nails - Burning Hot.</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xtz29rr8y3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>189de1x</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Not usually a dark polish gal but…</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189de1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>189cv6i</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>What vintage nail polish line do you still dream about? For me it's the Color Show collection from the 2010's and the Revlon Parfumerie collection also from the 2010's</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189cv6i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>189cprh</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Skipped the Coronation for a Presidential seat</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189cprh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>189bklv</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Please stare into the abyss of a useless screen with me. Issues with Lacquergram.</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/owcbljetrx3c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>189bjr0</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Capping short nails?</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/189bjr0/capping_short_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>189bibt</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Nails for my Mexican Vacation.</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivmlzvrarx3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>189bcch</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Space themed skittle 🪐👽🛸</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189bcch</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>189b8r4</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Matte Turquoise with Pink Shimmer</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jp7yqxq1px3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>189b84b</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Nail Shape Advice?</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189b84b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>189axpu</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Vent about previewed/actual polish colors and tips for color picking.</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/189axpu/vent_about_previewedactual_polish_colors_and_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>189askh</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Jade shorties</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189askh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>189apbi</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Sabertooth review</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/189apbi/sabertooth_review/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>189ali6</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Cirque 5 Days of Deals?</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/189ali6/cirque_5_days_of_deals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1899t22</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>I’ve joined the HoH gang—it’s so stunning</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1899t22</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1899ga1</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>🗑💚Oscar the Grouch💚🗑</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1899ga1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1899cat</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Ikea Helmer question</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1899cat/ikea_helmer_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>189979i</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>What is this nail polish?</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36o7dzwu7x3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1898px8</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>“Once Upon a Time” Vanessa Molina</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bw1wk6cs3x3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1898n48</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>First ILNP, and first flaky polish!</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1898n48</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1898fek</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Three coats Ethereal, Ether Dragon with a Bee’s Knees, Liar accent</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1898fek</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1898e9x</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Winter is here!</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f26e0uh21x3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>18983wq</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Not like the other reds :)</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tj88fadnyw3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1897v8v</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>My gel allergies will not stop me from using chrome powder. I've finally figured out how to use it with regular lacquer!</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1897v8v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1897o12</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Holotaco Wishlist</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1897o12/holotaco_wishlist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1897g7f</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Mooncat Not Today Satan</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fx8zy7v3tw3c1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1896f9m</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>ILNP “Bitten” is so underrated 🥵❤️🖤</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n9nprj33kw3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1894e9u</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Sparkly yule nails ❄️🌟</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.imgur.io/KkHnDEL.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>18936je</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Do you use 2 coats of top coat on all types of polish? Or only certain types (like glitter polish)?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/18936je/do_you_use_2_coats_of_top_coat_on_all_types_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1891hh1</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>I was worried this was going to look bad, but they turned out exactly as I hoped! 🎄</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1891hh1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1890ngb</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>In love with Mooncat Dragon Scales</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/omo8zxnuvu3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1890jmo</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Can anyone help me figure out what the name of this nail polish is?</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qclrd4ikuu3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1890iwk</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Near perfect Hydroflask match!</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1890iwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>18909n3</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>My first time trying Mooncat</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x93m9m9yqu3c1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>188zjia</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Cirque "Mobius" in velvet</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6cwuqfe9hu3c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>189kfly</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my mom's nails! </t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vay9awk2104c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>189kc32</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Black and gold winter nails</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rm4rs1xb004c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>189jcv7</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Blues Clues Winter 💙❄️</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fw59pzo8qz3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>189jaik</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>🇲🇽 Nail art by ig: @thewitch.nails</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189jaik</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>189igwp</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>First time painting someone else’s nails. She had TWO requests! Did I do her Justice???</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189igwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>189htss</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189htss</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>189ftfv</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>The Powerpuff Girls ❤️</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5a8yjs7hsy3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>189dimv</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Favorite holiday nails from last year!</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189dimv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>189bvkt</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>A couple holiday sets I’ve done so far.</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/189bvkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>189bbu3</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Dark nails</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b3qaipospx3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1899l2b</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>tortie nails</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzu2h34zax3c1.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1898kjx</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Any tips? :)</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1898kjx</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>